<commit_message>
db integration is partially complete
</commit_message>
<xml_diff>
--- a/archive/movies.xlsx
+++ b/archive/movies.xlsx
@@ -63,9 +63,6 @@
     <t>As Hollywood’s Golden Age is winding down during the summer of 1969, television actor Rick Dalton and his stunt double Cliff Booth endeavor to achieve lasting success in Hollywood while meeting several colorful characters along the way.</t>
   </si>
   <si>
-    <t>2019 • Comedy/Western • 2h 40m</t>
-  </si>
-  <si>
     <t>The Batman(2022)</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>When a sadistic serial killer begins murdering key political figures in Gotham, the Batman is forced to investigate the city's hidden corruption and question his family's involvement.</t>
   </si>
   <si>
-    <t>2022 • Action/Crime • 2h 56m</t>
-  </si>
-  <si>
     <t>Black Swan</t>
   </si>
   <si>
@@ -99,9 +93,6 @@
     <t>Nina is a talented but unstable ballerina on the verge of stardom. Pushed to the breaking point by her artistic director and a seductive rival, Nina's grip on reality slips, plunging her into a waking nightmare.</t>
   </si>
   <si>
-    <t>2010 • Horror/Drama • 1h 48m</t>
-  </si>
-  <si>
     <t>Inception</t>
   </si>
   <si>
@@ -114,9 +105,6 @@
     <t>A thief who steals corporate secrets through the use of dream-sharing technology is given the inverse task of planting an idea into the mind of a C.E.O., but his tragic past may doom the project and his team to disaster.</t>
   </si>
   <si>
-    <t>2010 • Sci-fi/Action • 2h 28m</t>
-  </si>
-  <si>
     <t>Barbie</t>
   </si>
   <si>
@@ -132,9 +120,6 @@
     <t>Barbie and Ken are having the time of their lives in the seemingly perfect world of Barbie Land. However, when they get a chance to go to the outside world, they soon discover the joys and perils of living among regular humans.</t>
   </si>
   <si>
-    <t>2023 • Comedy/Fantasy • 1h 54m</t>
-  </si>
-  <si>
     <t>Oppenheimerr</t>
   </si>
   <si>
@@ -147,9 +132,6 @@
     <t>A dramatization of the life story of J. Robert Oppenheimer, the physicist who had a large hand in the development of the atomic bombs that brought an end to World War II.</t>
   </si>
   <si>
-    <t>2023 • Drama/History • 3h</t>
-  </si>
-  <si>
     <t>The Long Shot</t>
   </si>
   <si>
@@ -165,9 +147,6 @@
     <t>Journalist, Fred Flarsky, reunites with his childhood crush, Charlotte Field; now one of the most influential women in the world. As she prepares to run for president, Charlotte hires Fred as her speechwriter, and sparks fly.</t>
   </si>
   <si>
-    <t>2019 • Comedy/Romance • 2h 5m</t>
-  </si>
-  <si>
     <t>3 Below: Tales of Arcadia</t>
   </si>
   <si>
@@ -180,9 +159,6 @@
     <t>A pair of teenage royals and their bodyguard escape from their home planet and try to blend in on Earth.</t>
   </si>
   <si>
-    <t>2018 • Sci-fi • 2 seasons</t>
-  </si>
-  <si>
     <t>The Prestige</t>
   </si>
   <si>
@@ -195,9 +171,6 @@
     <t>Rival 19th-century magicians engage in a bitter battle for trade secrets.</t>
   </si>
   <si>
-    <t>2006 • Thriller/Sci-fi • 2h 10m</t>
-  </si>
-  <si>
     <t>Interstellar</t>
   </si>
   <si>
@@ -210,9 +183,6 @@
     <t>When Earth becomes uninhabitable in the future, a farmer and ex-NASA pilot, Joseph Cooper, is tasked to pilot a spacecraft, along with a team of researchers, to find a new planet for humans.</t>
   </si>
   <si>
-    <t>2014 • Sci-fi/Adventure • 2h 49m</t>
-  </si>
-  <si>
     <t>Definitely, Maybe</t>
   </si>
   <si>
@@ -225,9 +195,6 @@
     <t>Set in New York City, the film is about a former political consultant who tries to help his daughter understand his impending divorce by telling her the story of his past romantic relationships and how he ended up marrying her mother. One of the best movies ever made.</t>
   </si>
   <si>
-    <t>2008 • Comedy/Romance • 1h 51m</t>
-  </si>
-  <si>
     <t>I Love You, Man</t>
   </si>
   <si>
@@ -246,9 +213,6 @@
     <t>movie_posters/download.jpeg</t>
   </si>
   <si>
-    <t>2009 • Comedy/Romance • 1h 45m</t>
-  </si>
-  <si>
     <t>Celeste And Jesse Forever</t>
   </si>
   <si>
@@ -267,9 +231,6 @@
     <t>movie_posters/download1.jpeg</t>
   </si>
   <si>
-    <t>2012 • Romance/Comedy • 1h 32m</t>
-  </si>
-  <si>
     <t>The Social Network</t>
   </si>
   <si>
@@ -279,9 +240,6 @@
     <t>Aaron Sorkin, Ben Mezrich</t>
   </si>
   <si>
-    <t>Jesse EisenbergAndrew GarfieldJustin Timberlake</t>
-  </si>
-  <si>
     <t>As Harvard student Mark Zuckerberg creates the social networking site that would become known as Facebook, he is sued by the twins who claimed he stole their idea and by the co-founder who was later squeezed out of the business.</t>
   </si>
   <si>
@@ -303,9 +261,6 @@
     <t>movie_posters/download2.jpeg</t>
   </si>
   <si>
-    <t>2019 • Family/Comedy • 1h 42m</t>
-  </si>
-  <si>
     <t>Inside Out</t>
   </si>
   <si>
@@ -315,21 +270,12 @@
     <t>Pete Docter, Ronnie Del Carmen, Meg LeFauve</t>
   </si>
   <si>
-    <t>Amy PoehlerBill HaderLewis Black</t>
-  </si>
-  <si>
     <t>After young Riley is uprooted from her Midwest life and moved to San Francisco, her emotions - Joy, Fear, Anger, Disgust and Sadness - conflict on how best to navigate a new city, house, and school.</t>
   </si>
   <si>
     <t>movie_posters/download3.jpeg</t>
   </si>
   <si>
-    <t>2015 • Family/Comedy • 1h 35m</t>
-  </si>
-  <si>
-    <t>2010 • Drama/Historical drama • 2 hours</t>
-  </si>
-  <si>
     <t>movie_posters/5.jpg</t>
   </si>
   <si>
@@ -361,6 +307,60 @@
   </si>
   <si>
     <t>movie_posters/11.jpg</t>
+  </si>
+  <si>
+    <t>Amy Poehler, Bill Hader, Lewis Black</t>
+  </si>
+  <si>
+    <t>Jesse Eisenberg, Andrew Garfield, Justin Timberlake</t>
+  </si>
+  <si>
+    <t>2019 | Comedy/Western | 2h 40m</t>
+  </si>
+  <si>
+    <t>2022 | Action/Crime | 2h 56m</t>
+  </si>
+  <si>
+    <t>2010 | Horror/Drama | 1h 48m</t>
+  </si>
+  <si>
+    <t>2010 | Sci-fi/Action | 2h 28m</t>
+  </si>
+  <si>
+    <t>2023 | Comedy/Fantasy | 1h 54m</t>
+  </si>
+  <si>
+    <t>2023 | Drama/History | 3h</t>
+  </si>
+  <si>
+    <t>2019 | Comedy/Romance | 2h 5m</t>
+  </si>
+  <si>
+    <t>2018 | Sci-fi | 2 seasons</t>
+  </si>
+  <si>
+    <t>2006 | Thriller/Sci-fi | 2h 10m</t>
+  </si>
+  <si>
+    <t>2014 | Sci-fi/Adventure | 2h 49m</t>
+  </si>
+  <si>
+    <t>2008 | Comedy/Romance | 1h 51m</t>
+  </si>
+  <si>
+    <t>2009 | Comedy/Romance | 1h 45m</t>
+  </si>
+  <si>
+    <t>2012 | Romance/Comedy | 1h 32m</t>
+  </si>
+  <si>
+    <t>2010 | Drama/Historical drama | 2 hours</t>
+  </si>
+  <si>
+    <t>2019 | Family/Comedy | 1h 42m</t>
+  </si>
+  <si>
+    <t>2015 | Family/Comedy | 1h 35m</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1170,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,10 +1238,10 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="I2">
         <v>8.9</v>
@@ -1255,25 +1255,25 @@
         <v>23456789</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
       <c r="G3" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="I3">
         <v>87</v>
@@ -1287,25 +1287,25 @@
         <v>34567890</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
       <c r="G4" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="I4">
         <v>9</v>
@@ -1319,25 +1319,25 @@
         <v>45678901</v>
       </c>
       <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
       <c r="G5" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="I5">
         <v>9.8000000000000007</v>
@@ -1351,25 +1351,25 @@
         <v>56789012</v>
       </c>
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
-      </c>
       <c r="G6" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>102</v>
       </c>
       <c r="I6">
         <v>120.1</v>
@@ -1383,25 +1383,25 @@
         <v>67890123</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G7" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="I7">
         <v>8.3000000000000007</v>
@@ -1415,25 +1415,25 @@
         <v>78901234</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="I8">
         <v>6.3</v>
@@ -1447,25 +1447,25 @@
         <v>89012345</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="I9">
         <v>9.5</v>
@@ -1479,25 +1479,25 @@
         <v>90123456</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="H10" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="I10">
         <v>9.9</v>
@@ -1511,25 +1511,25 @@
         <v>12345670</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="I11">
         <v>8.6999999999999993</v>
@@ -1543,25 +1543,25 @@
         <v>12345610</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="G12" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="I12">
         <v>37.5</v>
@@ -1575,25 +1575,25 @@
         <v>25584819</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F13" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G13" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="I13">
         <v>7</v>
@@ -1607,25 +1607,25 @@
         <v>13745536</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G14" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="I14">
         <v>6.6</v>
@@ -1639,25 +1639,25 @@
         <v>65794022</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="F15" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G15" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="H15" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="I15">
         <v>7.8</v>
@@ -1671,25 +1671,25 @@
         <v>84299799</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="H16" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="I16">
         <v>6.8</v>
@@ -1703,25 +1703,25 @@
         <v>91129071</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" t="s">
         <v>96</v>
       </c>
-      <c r="D17" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" t="s">
-        <v>98</v>
-      </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="G17" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="H17" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="I17">
         <v>8.1</v>

</xml_diff>